<commit_message>
tacluso cyn yr eisteddfod
</commit_message>
<xml_diff>
--- a/data/ebrydydd_data.xlsx
+++ b/data/ebrydydd_data.xlsx
@@ -1309,9 +1309,6 @@
     <t>d/h-yn-ateb-c</t>
   </si>
   <si>
-    <t>g/rh-yn-ateb-cr</t>
-  </si>
-  <si>
     <t>Diwedd i fyd dydd y Farn</t>
   </si>
   <si>
@@ -1385,6 +1382,9 @@
   </si>
   <si>
     <t>g/g-yn-ateb-g</t>
+  </si>
+  <si>
+    <t>g/rh-yn-ateb-c/r</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>109</v>
@@ -3882,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4411,7 +4411,7 @@
         <v>117</v>
       </c>
       <c r="G33" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -4573,7 +4573,7 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C55" t="s">
         <v>49</v>
@@ -4679,7 +4679,7 @@
         <v>117</v>
       </c>
       <c r="G55" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -4704,7 +4704,7 @@
         <v>117</v>
       </c>
       <c r="G57" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -4737,7 +4737,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C60" t="s">
         <v>49</v>
@@ -4746,7 +4746,7 @@
         <v>117</v>
       </c>
       <c r="G60" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -4762,7 +4762,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C62" t="s">
         <v>49</v>
@@ -4771,7 +4771,7 @@
         <v>117</v>
       </c>
       <c r="G62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -4834,7 +4834,7 @@
         <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F68" t="s">
         <v>117</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C73" t="s">
         <v>22</v>
@@ -4898,12 +4898,12 @@
         <v>117</v>
       </c>
       <c r="G73" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C74" t="s">
         <v>22</v>
@@ -4912,12 +4912,12 @@
         <v>117</v>
       </c>
       <c r="G74" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C75" t="s">
         <v>22</v>
@@ -4926,12 +4926,12 @@
         <v>117</v>
       </c>
       <c r="G75" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C76" t="s">
         <v>21</v>
@@ -4940,12 +4940,12 @@
         <v>117</v>
       </c>
       <c r="G76" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C77" t="s">
         <v>22</v>
@@ -4954,12 +4954,12 @@
         <v>117</v>
       </c>
       <c r="G77" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C78" t="s">
         <v>22</v>
@@ -4968,12 +4968,12 @@
         <v>117</v>
       </c>
       <c r="G78" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C79" t="s">
         <v>22</v>
@@ -4982,7 +4982,7 @@
         <v>117</v>
       </c>
       <c r="G79" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -5215,7 +5215,7 @@
         <v>117</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>

</xml_diff>